<commit_message>
Comitted by Pratik on 30 Sept
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/TestDataExcel.xlsx
+++ b/src/main/java/TestData/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pshinde6\eclipse-workspace\Health\src\main\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA3554D-A434-44A8-9E62-2D2D209FD93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9832979-59B8-4597-9ABA-153AD04A61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{958C6FBC-916B-4DAF-8B01-40ACC92B8EF9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Shinde</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>IsSelfIncluded</t>
   </si>
   <si>
@@ -131,16 +128,108 @@
   </si>
   <si>
     <t>DOBFatherInLaw</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>13/11/1992</t>
+  </si>
+  <si>
+    <t>SISelf</t>
+  </si>
+  <si>
+    <t>SISpouse</t>
+  </si>
+  <si>
+    <t>SIFather</t>
+  </si>
+  <si>
+    <t>SIMother</t>
+  </si>
+  <si>
+    <t>SISon</t>
+  </si>
+  <si>
+    <t>SIDaughter</t>
+  </si>
+  <si>
+    <t>SIFatherInLaw</t>
+  </si>
+  <si>
+    <t>SIMotherInLaw</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>NumberOfInsureds</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>24/06/1980</t>
+  </si>
+  <si>
+    <t>Medicare Premier</t>
+  </si>
+  <si>
+    <t>Varient</t>
+  </si>
+  <si>
+    <t>CustTitle</t>
+  </si>
+  <si>
+    <t>CustFirstName</t>
+  </si>
+  <si>
+    <t>CustMiddleName</t>
+  </si>
+  <si>
+    <t>CustLastName</t>
+  </si>
+  <si>
+    <t>CustEmailID</t>
+  </si>
+  <si>
+    <t>CustMobileNo</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>pratik.qualitykiosk@tataaig.com</t>
+  </si>
+  <si>
+    <t>ConvertToPropsal</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,19 +252,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,40 +585,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A133093E-F5DF-46C1-966C-BAAC8B52A6CF}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="2"/>
     <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="2"/>
     <col min="21" max="21" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="18.7109375" style="2"/>
+    <col min="24" max="24" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="45" width="20.5703125" style="2" customWidth="1"/>
+    <col min="46" max="16384" width="8.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,64 +649,112 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>30</v>
+      <c r="X1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -605,10 +767,86 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="3">
+        <v>33919</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>8356809451</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AK2" r:id="rId1" xr:uid="{9CBADEC4-0465-4DE7-AEE8-2895A65E2209}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -617,10 +855,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -649,9 +893,7 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2">
         <v>123</v>
       </c>

</xml_diff>